<commit_message>
Check that thought about char. pixel recovery's working starting from 0.
</commit_message>
<xml_diff>
--- a/refFiles/mx_manip/posRecovery()_StartingFrom0.xlsx
+++ b/refFiles/mx_manip/posRecovery()_StartingFrom0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FilpUsine1\Documents\dev-ws2812b\refFiles\mx_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FAC730-BBF0-4C98-A89E-E7F4F7D5D09B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE27267-89CC-49A7-B1D5-A8984107D18B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="630" windowWidth="38700" windowHeight="15435" activeTab="4" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
+    <workbookView xWindow="45" yWindow="630" windowWidth="38700" windowHeight="15435" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
   </bookViews>
   <sheets>
     <sheet name="0_360" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>Simple Matrix</t>
   </si>
@@ -83,18 +83,6 @@
   </si>
   <si>
     <t>Multiple Matrixes (NEXT to each others)</t>
-  </si>
-  <si>
-    <t>(X / (MAX_COLU + 1)) * MAX_LEDS + (MAX_COLU - (X % 17)) + (Y - 1) * MAX_COLU</t>
-  </si>
-  <si>
-    <t>(X / (MAX_COLU + 1)) * MAX_LEDS + ((X % 17) - 1)                      + (Y - 1) * MAX_COLU</t>
-  </si>
-  <si>
-    <t>To debug ...</t>
-  </si>
-  <si>
-    <t>Don't work properly with X &gt; 16</t>
   </si>
   <si>
     <t>i &lt;- 0 to MAX_LINE</t>
@@ -144,6 +132,30 @@
   <si>
     <t>X * MAX_LINE + Y</t>
   </si>
+  <si>
+    <t>X / MAX_COL * MXA_LEDS + X % MAX_COL + Y * MAX_COL</t>
+  </si>
+  <si>
+    <t>X / MAX_COL * MXA_LEDS + (Y + 1) * MAX_COLU - X % 16- 1</t>
+  </si>
+  <si>
+    <t>X / MAX_COL * MXA_LEDS + MAX_LEDS - X % MAX_COL * MAX_LINE - Y - 1</t>
+  </si>
+  <si>
+    <t>28 pixels</t>
+  </si>
+  <si>
+    <t>LINE</t>
+  </si>
+  <si>
+    <t>COLUMN</t>
+  </si>
+  <si>
+    <t>Pixel pos.</t>
+  </si>
+  <si>
+    <t>i in Array</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,21 +261,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -285,6 +311,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -628,11 +664,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5B93D0-ABDB-40CB-8D7C-2E1071F7F2BA}">
-  <dimension ref="A1:AQ37"/>
+  <dimension ref="A1:AQ32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -807,7 +841,7 @@
         <v>7</v>
       </c>
       <c r="AO2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -947,7 +981,7 @@
       <c r="AM3" s="4"/>
       <c r="AN3" s="14"/>
       <c r="AP3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1085,7 +1119,7 @@
       <c r="AM4" s="4"/>
       <c r="AN4" s="14"/>
       <c r="AQ4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -2917,20 +2951,20 @@
       </c>
       <c r="F24" s="2">
         <f>IF(MOD(C25, 2) = 0, C24 + C25 * D19, (C25 + 1) * D19 - C24 - 1)</f>
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="T24" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="V24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="W24" s="2">
         <f xml:space="preserve"> IF(MOD(T25, 2) = 0, T29, T32)</f>
-        <v>240</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.25">
@@ -2938,13 +2972,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="T25" s="2">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.25">
@@ -2957,10 +2991,10 @@
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.25">
@@ -2968,13 +3002,13 @@
         <v>8</v>
       </c>
       <c r="T29" s="2">
-        <f xml:space="preserve"> INT((T24 / (D19 + 1))) * H19 + (D19 - MOD(T24, 17)) + (T25 - 1) * D19</f>
-        <v>240</v>
+        <f xml:space="preserve"> INT(T24 / D19) * H19 + MOD(T24, D19) + T25 * D19</f>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>8</v>
@@ -2982,23 +3016,13 @@
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.25">
       <c r="T31" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:34" x14ac:dyDescent="0.25">
       <c r="T32" s="2">
-        <f xml:space="preserve"> INT((T24 /(D19 + 1))) * H19 + (MOD(T24,17) - 1) + (T25 - 1) * D19</f>
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="20:20" x14ac:dyDescent="0.25">
-      <c r="T36" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="20:20" x14ac:dyDescent="0.25">
-      <c r="T37" s="2" t="s">
-        <v>18</v>
+        <f xml:space="preserve"> INT(T24 / D19) * H19 + (T25 + 1) * D19 - MOD(T24,D19) - 1</f>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3024,11 +3048,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFE2C2D-56A6-462B-9FCF-1302A82E64E8}">
-  <dimension ref="A1:AN30"/>
+  <dimension ref="A1:AN31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5219,20 +5241,27 @@
         <v>2</v>
       </c>
       <c r="C24" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="2">
         <f>IF(MOD(C24, 2) = 0, H19 - C24 * D20 - C25 - 1, H19 - (C24 + 1) * D20 + C25)</f>
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="T24" s="2">
+        <v>20</v>
+      </c>
       <c r="V24" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="W24" s="2">
+        <f>IF(MOD(T24,2) = 0,T29,T32)</f>
+        <v>507</v>
       </c>
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.25">
@@ -5240,10 +5269,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="T25" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.25">
@@ -5251,28 +5283,48 @@
         <v>9</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="T29" s="2">
+        <f xml:space="preserve"> (T24 / D19 * H19) + H19 - (MOD(T24,D19) * D20) - T25 - 1</f>
+        <v>507</v>
+      </c>
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="T31" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$F$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:Q17 S2:AH17">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>$W$24</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5284,9 +5336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688FCD4D-605E-4791-BC54-A6D9EB8A5096}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7470,7 +7520,7 @@
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.25">
@@ -7480,12 +7530,12 @@
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7498,9 +7548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF87678-2DC5-468A-BDD2-E206238D660F}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9684,7 +9732,7 @@
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.25">
@@ -9694,12 +9742,12 @@
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9710,11 +9758,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D21C5-C0A1-4E54-8694-7F6956E417E2}">
-  <dimension ref="A1:AQ25"/>
+  <dimension ref="A1:AQ56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9727,7 +9773,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
+      <c r="B1" s="21" t="str">
+        <f>"Result : "&amp;O25&amp;", "&amp;O26&amp;", "&amp;O27&amp;", "&amp;O28&amp;" - "&amp;O29&amp;", "&amp;O30&amp;", "&amp;O31&amp;", "&amp;O32&amp;" - "&amp;O33&amp;", "&amp;O34&amp;", "&amp;O35&amp;", "&amp;O36&amp;" - "&amp;O37&amp;", "&amp;O38&amp;", "&amp;O39&amp;", "&amp;O40&amp;" - "&amp;O41&amp;", "&amp;O42&amp;", "&amp;O43&amp;", "&amp;O44&amp;" - "&amp;O45&amp;", "&amp;O46&amp;", "&amp;O47&amp;", "&amp;O48&amp;" - "&amp;O49&amp;", "&amp;O50&amp;", "&amp;O51&amp;", "&amp;O52</f>
+        <v>Result : 125, 124, 123, 122 - 130, 131, 132, 133 - 157, 156, 155, 154 - 162, 163, 164, 165 - 189, 188, 187, 186 - 194, 195, 196, 197 - 221, 220, 219, 218</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -9826,7 +9875,7 @@
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
@@ -9921,7 +9970,7 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -10013,7 +10062,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -10104,7 +10153,7 @@
       <c r="W5" s="14"/>
       <c r="X5" s="1"/>
       <c r="Z5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -10195,7 +10244,7 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
@@ -11196,8 +11245,11 @@
       <c r="AH17" s="1"/>
     </row>
     <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="S18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="T18"/>
       <c r="U18"/>
@@ -11205,50 +11257,567 @@
       <c r="W18" s="1"/>
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>16</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2">
+        <v>256</v>
+      </c>
       <c r="S19"/>
       <c r="T19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="U19"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2">
+        <v>16</v>
+      </c>
       <c r="S20"/>
       <c r="T20"/>
       <c r="U20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
     </row>
+    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="24" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2">
+        <f>IF(MOD(C25, 2) = 0, C24 + C25 * D19, (C25 + 1) * D19 - C24 - 1)</f>
+        <v>125</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="S24" s="3"/>
       <c r="V24" s="3"/>
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7</v>
+      </c>
+      <c r="J25" s="18">
+        <v>0</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
+        <v>0</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19">
+        <f>IF(MOD(C$25 + J$25, 2) = 0, C$24 + L25 + (C$25 + J$25) * D$19, (C$25 + J$25 + 1) * D$19 - C$24 - L25 - 1)</f>
+        <v>125</v>
+      </c>
+      <c r="R25" s="19">
+        <f>L25 + J$25 * S$9</f>
+        <v>0</v>
+      </c>
       <c r="S25" s="3"/>
     </row>
+    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
+        <v>1</v>
+      </c>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19">
+        <f t="shared" ref="O26:O28" si="15">IF(MOD(C$25 + J$25, 2) = 0, C$24 + L26 + (C$25 + J$25) * D$19, (C$25 + J$25 + 1) * D$19 - C$24 - L26 - 1)</f>
+        <v>124</v>
+      </c>
+      <c r="R26" s="19">
+        <f t="shared" ref="R26:R28" si="16">L26 + J$25 * S$9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J27" s="18"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
+        <v>2</v>
+      </c>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19">
+        <f t="shared" si="15"/>
+        <v>123</v>
+      </c>
+      <c r="R27" s="19">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J28" s="18"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19">
+        <v>3</v>
+      </c>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19">
+        <f t="shared" si="15"/>
+        <v>122</v>
+      </c>
+      <c r="R28" s="19">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J29" s="16">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+      <c r="O29" s="20">
+        <f>IF(MOD(C$25 + J$29, 2) = 0, C$24 + L29 + (C$25 + J$29) * D$19, (C$25 + J$29 + 1) * D$19 - C$24 - L29 - 1)</f>
+        <v>130</v>
+      </c>
+      <c r="R29" s="2">
+        <f>L29 + J$29 * S$9</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J30" s="16"/>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="20">
+        <f t="shared" ref="O30:O32" si="17">IF(MOD(C$25 + J$29, 2) = 0, C$24 + L30 + (C$25 + J$29) * D$19, (C$25 + J$29 + 1) * D$19 - C$24 - L30 - 1)</f>
+        <v>131</v>
+      </c>
+      <c r="R30" s="2">
+        <f t="shared" ref="R30:R32" si="18">L30 + J$29 * S$9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J31" s="16"/>
+      <c r="L31" s="2">
+        <v>2</v>
+      </c>
+      <c r="O31" s="20">
+        <f t="shared" si="17"/>
+        <v>132</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J32" s="16"/>
+      <c r="L32" s="2">
+        <v>3</v>
+      </c>
+      <c r="O32" s="20">
+        <f t="shared" si="17"/>
+        <v>133</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J33" s="18">
+        <v>2</v>
+      </c>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19">
+        <v>0</v>
+      </c>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19">
+        <f>IF(MOD(C$25 + J$33, 2) = 0, C$24 + L33 + (C$25 + J$33) * D$19, (C$25 + J$33 + 1) * D$19 - C$24 - L33 - 1)</f>
+        <v>157</v>
+      </c>
+      <c r="R33" s="19">
+        <f>L33 + J$33 * S$9</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J34" s="18"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19">
+        <v>1</v>
+      </c>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19">
+        <f t="shared" ref="O34:O37" si="19">IF(MOD(C$25 + J$33, 2) = 0, C$24 + L34 + (C$25 + J$33) * D$19, (C$25 + J$33 + 1) * D$19 - C$24 - L34 - 1)</f>
+        <v>156</v>
+      </c>
+      <c r="R34" s="19">
+        <f t="shared" ref="R34:R36" si="20">L34 + J$33 * S$9</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J35" s="18"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19">
+        <v>2</v>
+      </c>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19">
+        <f t="shared" si="19"/>
+        <v>155</v>
+      </c>
+      <c r="R35" s="19">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J36" s="18"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19">
+        <v>3</v>
+      </c>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19">
+        <f t="shared" si="19"/>
+        <v>154</v>
+      </c>
+      <c r="R36" s="19">
+        <f t="shared" si="20"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J37" s="16">
+        <v>3</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="O37" s="20">
+        <f>IF(MOD(C$25 + J$37, 2) = 0, C$24 + L37 + (C$25 + J$37) * D$19, (C$25 + J$37 + 1) * D$19 - C$24 - L37 - 1)</f>
+        <v>162</v>
+      </c>
+      <c r="R37" s="2">
+        <f>L37 + J$37 * S$9</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J38" s="16"/>
+      <c r="L38" s="2">
+        <v>1</v>
+      </c>
+      <c r="O38" s="20">
+        <f t="shared" ref="O38:O40" si="21">IF(MOD(C$25 + J$37, 2) = 0, C$24 + L38 + (C$25 + J$37) * D$19, (C$25 + J$37 + 1) * D$19 - C$24 - L38 - 1)</f>
+        <v>163</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" ref="R38:R40" si="22">L38 + J$37 * S$9</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J39" s="16"/>
+      <c r="L39" s="2">
+        <v>2</v>
+      </c>
+      <c r="O39" s="20">
+        <f t="shared" si="21"/>
+        <v>164</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="22"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J40" s="16"/>
+      <c r="L40" s="2">
+        <v>3</v>
+      </c>
+      <c r="O40" s="20">
+        <f t="shared" si="21"/>
+        <v>165</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="22"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J41" s="18">
+        <v>4</v>
+      </c>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19">
+        <v>0</v>
+      </c>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19">
+        <f>IF(MOD(C$25 + J$41, 2) = 0, C$24 + L41 + (C$25 + J$41) * D$19, (C$25 + J$41 + 1) * D$19 - C$24 - L41 - 1)</f>
+        <v>189</v>
+      </c>
+      <c r="R41" s="19">
+        <f>L41 + J$41 * S$9</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J42" s="18"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19">
+        <v>1</v>
+      </c>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19">
+        <f t="shared" ref="O42:O44" si="23">IF(MOD(C$25 + J$41, 2) = 0, C$24 + L42 + (C$25 + J$41) * D$19, (C$25 + J$41 + 1) * D$19 - C$24 - L42 - 1)</f>
+        <v>188</v>
+      </c>
+      <c r="R42" s="19">
+        <f t="shared" ref="R42:R44" si="24">L42 + J$41 * S$9</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J43" s="18"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19">
+        <v>2</v>
+      </c>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19">
+        <f t="shared" si="23"/>
+        <v>187</v>
+      </c>
+      <c r="R43" s="19">
+        <f t="shared" si="24"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J44" s="18"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19">
+        <v>3</v>
+      </c>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19">
+        <f t="shared" si="23"/>
+        <v>186</v>
+      </c>
+      <c r="R44" s="19">
+        <f t="shared" si="24"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J45" s="16">
+        <v>5</v>
+      </c>
+      <c r="L45" s="2">
+        <v>0</v>
+      </c>
+      <c r="O45" s="20">
+        <f>IF(MOD(C$25 + J$45, 2) = 0, C$24 + L45 + (C$25 + J$45) * D$19, (C$25 + J$45 + 1) * D$19 - C$24 - L45 - 1)</f>
+        <v>194</v>
+      </c>
+      <c r="R45" s="2">
+        <f>L45 + J$45 * S$9</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J46" s="16"/>
+      <c r="L46" s="2">
+        <v>1</v>
+      </c>
+      <c r="O46" s="20">
+        <f t="shared" ref="O46:O48" si="25">IF(MOD(C$25 + J$45, 2) = 0, C$24 + L46 + (C$25 + J$45) * D$19, (C$25 + J$45 + 1) * D$19 - C$24 - L46 - 1)</f>
+        <v>195</v>
+      </c>
+      <c r="R46" s="2">
+        <f t="shared" ref="R46:R48" si="26">L46 + J$45 * S$9</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J47" s="16"/>
+      <c r="L47" s="2">
+        <v>2</v>
+      </c>
+      <c r="O47" s="20">
+        <f t="shared" si="25"/>
+        <v>196</v>
+      </c>
+      <c r="R47" s="2">
+        <f t="shared" si="26"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J48" s="16"/>
+      <c r="L48" s="2">
+        <v>3</v>
+      </c>
+      <c r="O48" s="20">
+        <f t="shared" si="25"/>
+        <v>197</v>
+      </c>
+      <c r="R48" s="2">
+        <f t="shared" si="26"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J49" s="18">
+        <v>6</v>
+      </c>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19">
+        <v>0</v>
+      </c>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19">
+        <f>IF(MOD(C$25 + J$49, 2) = 0, C$24 + L49 + (C$25 + J$49) * D$19, (C$25 + J$49 + 1) * D$19 - C$24 - L49 - 1)</f>
+        <v>221</v>
+      </c>
+      <c r="R49" s="19">
+        <f>L49 + J$49 * S$9</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J50" s="18"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19">
+        <v>1</v>
+      </c>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19">
+        <f t="shared" ref="O50:O52" si="27">IF(MOD(C$25 + J$49, 2) = 0, C$24 + L50 + (C$25 + J$49) * D$19, (C$25 + J$49 + 1) * D$19 - C$24 - L50 - 1)</f>
+        <v>220</v>
+      </c>
+      <c r="R50" s="19">
+        <f t="shared" ref="R50:R52" si="28">L50 + J$49 * S$9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J51" s="18"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19">
+        <v>2</v>
+      </c>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19">
+        <f t="shared" si="27"/>
+        <v>219</v>
+      </c>
+      <c r="R51" s="19">
+        <f t="shared" si="28"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J52" s="18"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19">
+        <v>3</v>
+      </c>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19">
+        <f t="shared" si="27"/>
+        <v>218</v>
+      </c>
+      <c r="R52" s="19">
+        <f t="shared" si="28"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J53" s="17"/>
+    </row>
+    <row r="54" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J54" s="17"/>
+    </row>
+    <row r="55" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J55" s="17"/>
+    </row>
+    <row r="56" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J56" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="10">
+    <mergeCell ref="J33:J36"/>
+    <mergeCell ref="J37:J40"/>
+    <mergeCell ref="J41:J44"/>
+    <mergeCell ref="J45:J48"/>
+    <mergeCell ref="J49:J52"/>
     <mergeCell ref="W2:W8"/>
     <mergeCell ref="S9:V9"/>
     <mergeCell ref="W10:W16"/>
+    <mergeCell ref="J25:J28"/>
+    <mergeCell ref="J29:J32"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>$F$24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>$W$24</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>